<commit_message>
Fixed the colors in the excel graph. Added descriptions for building and calibrating.
</commit_message>
<xml_diff>
--- a/documentation/ColorCurve-PWM-levels.xlsx
+++ b/documentation/ColorCurve-PWM-levels.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="19000" tabRatio="500"/>
@@ -136,6 +136,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -221,6 +228,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -306,6 +320,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -387,11 +408,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134349624"/>
-        <c:axId val="2134550344"/>
+        <c:axId val="2119569464"/>
+        <c:axId val="2119572440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134349624"/>
+        <c:axId val="2119569464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -401,7 +422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134550344"/>
+        <c:crossAx val="2119572440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -409,7 +430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134550344"/>
+        <c:axId val="2119572440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,7 +441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134349624"/>
+        <c:crossAx val="2119569464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -802,7 +823,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -832,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>1000*A2/7</f>
+        <f t="shared" ref="E2:E9" si="0">1000*A2/7</f>
         <v>0</v>
       </c>
     </row>
@@ -850,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f>1000*A3/7</f>
+        <f t="shared" si="0"/>
         <v>142.85714285714286</v>
       </c>
     </row>
@@ -868,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <f>1000*A4/7</f>
+        <f t="shared" si="0"/>
         <v>285.71428571428572</v>
       </c>
     </row>
@@ -886,7 +907,7 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <f>1000*A5/7</f>
+        <f t="shared" si="0"/>
         <v>428.57142857142856</v>
       </c>
     </row>
@@ -904,7 +925,7 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <f>1000*A6/7</f>
+        <f t="shared" si="0"/>
         <v>571.42857142857144</v>
       </c>
     </row>
@@ -922,7 +943,7 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <f>1000*A7/7</f>
+        <f t="shared" si="0"/>
         <v>714.28571428571433</v>
       </c>
     </row>
@@ -940,7 +961,7 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <f>1000*A8/7</f>
+        <f t="shared" si="0"/>
         <v>857.14285714285711</v>
       </c>
     </row>
@@ -958,7 +979,7 @@
         <v>76</v>
       </c>
       <c r="E9">
-        <f>1000*A9/7</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>

</xml_diff>